<commit_message>
adding job and param file maker
</commit_message>
<xml_diff>
--- a/source_models/zones/2018_mw/oq_job_tracking.xlsx
+++ b/source_models/zones/2018_mw/oq_job_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tallen/Documents/Geoscience_Australia/NSHA2018/source_models/zones/2018_mw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DB9C35-8B26-114F-AAD5-63A171729B4F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99BE3C50-8286-A04E-8992-C8215445AD62}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="28680" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,11 +18,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Run</t>
   </si>
@@ -42,12 +43,6 @@
     <t>Result</t>
   </si>
   <si>
-    <t>oq512c512h</t>
-  </si>
-  <si>
-    <t>oq512c512ht</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -82,6 +77,9 @@
   </si>
   <si>
     <t>Site Discretisation</t>
+  </si>
+  <si>
+    <t>PGA</t>
   </si>
 </sst>
 </file>
@@ -467,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -498,36 +496,33 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
         <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>0.33333333333333331</v>
@@ -553,10 +548,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>0.66666666666666663</v>
@@ -580,7 +572,7 @@
         <v>9.4</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K3">
         <v>500</v>
@@ -591,9 +583,6 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1">
@@ -618,7 +607,7 @@
         <v>500</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M4">
         <v>10</v>
@@ -626,7 +615,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>0.66666666666666663</v>
@@ -639,6 +628,9 @@
       </c>
       <c r="G5">
         <v>500</v>
+      </c>
+      <c r="I5" s="3">
+        <v>16</v>
       </c>
       <c r="M5">
         <v>10</v>
@@ -646,7 +638,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>0.66666666666666663</v>
@@ -666,6 +658,47 @@
       </c>
       <c r="M6">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>5039046</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D7" s="4">
+        <v>256</v>
+      </c>
+      <c r="E7">
+        <v>512</v>
+      </c>
+      <c r="F7">
+        <v>54</v>
+      </c>
+      <c r="G7">
+        <v>200</v>
+      </c>
+      <c r="H7">
+        <v>4.5</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating nsha13 background model
</commit_message>
<xml_diff>
--- a/source_models/zones/2018_mw/oq_job_tracking.xlsx
+++ b/source_models/zones/2018_mw/oq_job_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tallen/Documents/Geoscience_Australia/NSHA2018/source_models/zones/2018_mw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99BE3C50-8286-A04E-8992-C8215445AD62}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F03DBBE-C88B-3A42-A320-5BF879C384DF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="28680" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Run</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>PGA</t>
+  </si>
+  <si>
+    <t>All T</t>
+  </si>
+  <si>
+    <t>csv</t>
   </si>
 </sst>
 </file>
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -545,6 +551,9 @@
       <c r="K2">
         <v>500</v>
       </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -577,6 +586,9 @@
       <c r="K3">
         <v>500</v>
       </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
       <c r="M3">
         <v>15</v>
       </c>
@@ -632,6 +644,9 @@
       <c r="I5" s="3">
         <v>16</v>
       </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
       <c r="M5">
         <v>10</v>
       </c>
@@ -656,6 +671,9 @@
       <c r="K6">
         <v>0</v>
       </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
       <c r="M6">
         <v>10</v>
       </c>
@@ -697,8 +715,54 @@
       <c r="L7" t="s">
         <v>18</v>
       </c>
-      <c r="M7">
-        <v>15</v>
+      <c r="M7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="D8">
+        <v>256</v>
+      </c>
+      <c r="E8">
+        <v>256</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="D9">
+        <v>256</v>
+      </c>
+      <c r="E9">
+        <v>256</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>